<commit_message>
Lock on data dictionary
</commit_message>
<xml_diff>
--- a/www/data-entry-template/GLATAR_data_entry_template_v15.xlsx
+++ b/www/data-entry-template/GLATAR_data_entry_template_v15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benhlina/Library/CloudStorage/Dropbox/GitHub/GLATAR-App/www/data-entry-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1CA81F-0276-6946-A9AD-1ED1F9640A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59ABC61-42F1-BB4F-82B5-B738E9939511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19460" activeTab="2" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19460" xr2:uid="{DE6F8925-643B-304C-8933-23D4A9123DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -1660,7 +1660,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
@@ -2722,7 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422A67CE-83F0-2A4B-88E8-E8A3F38049A2}">
   <dimension ref="A1:O10226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="134" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>